<commit_message>
csv for some of them
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dead to Me/deadtome.xlsx
+++ b/Assets/Resources/Dead to Me/deadtome.xlsx
@@ -5,36 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\Songs\Dead To Me (Instrumental)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rhythm-Road\Rhythm-Road\Assets\Resources\Dead to Me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183C19C4-5F57-427F-B5E3-61AE37993F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0065BE8-F1A6-414B-9FC7-0A16F919D41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="greatdays" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="1">
   <si>
     <t>N</t>
   </si>
@@ -877,17 +864,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>25934</v>
+        <v>2015</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -896,13 +883,13 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <f>A1/1000</f>
-        <v>25.934000000000001</v>
+        <f t="shared" ref="D1:D49" si="0">A1/1000</f>
+        <v>2.0150000000000001</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>26745</v>
+        <v>2421</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -911,55 +898,55 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D65" si="0">A2/1000</f>
-        <v>26.745000000000001</v>
+        <f t="shared" si="0"/>
+        <v>2.4209999999999998</v>
       </c>
       <c r="E2">
-        <f>D2-D1</f>
-        <v>0.81099999999999994</v>
+        <f t="shared" ref="E2:E50" si="1">D2-D1</f>
+        <v>0.40599999999999969</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>29177</v>
+        <v>2691</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>29.177</v>
+        <v>2.6909999999999998</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="1">D3-D2</f>
-        <v>2.4319999999999986</v>
+        <f t="shared" si="1"/>
+        <v>0.27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>29988</v>
+        <v>2826</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>29.988</v>
+        <v>2.8260000000000001</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>0.81099999999999994</v>
+        <v>0.13500000000000023</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>30799</v>
+        <v>3096</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -969,73 +956,73 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>30.798999999999999</v>
+        <v>3.0960000000000001</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>0.81099999999999994</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>31475</v>
+        <v>3231</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>31.475000000000001</v>
+        <v>3.2309999999999999</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>0.67600000000000193</v>
+        <v>0.13499999999999979</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>32421</v>
+        <v>3502</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>32.420999999999999</v>
+        <v>3.5019999999999998</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0.94599999999999795</v>
+        <v>0.27099999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>33907</v>
+        <v>4853</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>33.906999999999996</v>
+        <v>4.8529999999999998</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>1.4859999999999971</v>
+        <v>1.351</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>35664</v>
+        <v>5258</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -1045,54 +1032,54 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>35.664000000000001</v>
+        <v>5.258</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>1.757000000000005</v>
+        <v>0.40500000000000025</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>36475</v>
+        <v>6475</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>36.475000000000001</v>
+        <v>6.4749999999999996</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.81099999999999994</v>
+        <v>1.2169999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>40529</v>
+        <v>7150</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>40.529000000000003</v>
+        <v>7.15</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>4.054000000000002</v>
+        <v>0.67500000000000071</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>42015</v>
+        <v>8096</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -1102,16 +1089,16 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>42.015000000000001</v>
+        <v>8.0960000000000001</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>1.4859999999999971</v>
+        <v>0.94599999999999973</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>42150</v>
+        <v>8502</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1121,54 +1108,54 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>42.15</v>
+        <v>8.5020000000000007</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>0.13499999999999801</v>
+        <v>0.40600000000000058</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>43772</v>
+        <v>8907</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>43.771999999999998</v>
+        <v>8.907</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>1.6219999999999999</v>
+        <v>0.40499999999999936</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>44448</v>
+        <v>9177</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>44.448</v>
+        <v>9.1769999999999996</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>0.67600000000000193</v>
+        <v>0.26999999999999957</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>45258</v>
+        <v>9312</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -1178,16 +1165,16 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>45.258000000000003</v>
+        <v>9.3119999999999994</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>0.81000000000000227</v>
+        <v>0.13499999999999979</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>45394</v>
+        <v>9448</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1197,54 +1184,54 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>45.393999999999998</v>
+        <v>9.4480000000000004</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>0.13599999999999568</v>
+        <v>0.13600000000000101</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>46204</v>
+        <v>9583</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>46.204000000000001</v>
+        <v>9.5830000000000002</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>0.81000000000000227</v>
+        <v>0.13499999999999979</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>46475</v>
+        <v>9718</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>46.475000000000001</v>
+        <v>9.718</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>0.2710000000000008</v>
+        <v>0.13499999999999979</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>47015</v>
+        <v>10664</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -1254,111 +1241,111 @@
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>47.015000000000001</v>
+        <v>10.664</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>0.53999999999999915</v>
+        <v>0.94599999999999973</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>48502</v>
+        <v>10799</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>48.502000000000002</v>
+        <v>10.798999999999999</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>1.4870000000000019</v>
+        <v>0.13499999999999979</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>48637</v>
+        <v>11610</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>48.637</v>
+        <v>11.61</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>0.13499999999999801</v>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>50258</v>
+        <v>11745</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>50.258000000000003</v>
+        <v>11.744999999999999</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>1.6210000000000022</v>
+        <v>0.13499999999999979</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>50934</v>
+        <v>13096</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>50.933999999999997</v>
+        <v>13.096</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>0.67599999999999483</v>
+        <v>1.3510000000000009</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>51880</v>
+        <v>13907</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>51.88</v>
+        <v>13.907</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>0.94600000000000506</v>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>52285</v>
+        <v>14312</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1368,121 +1355,121 @@
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>52.284999999999997</v>
+        <v>14.311999999999999</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>0.40499999999999403</v>
+        <v>0.40499999999999936</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>55123</v>
+        <v>14718</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>55.122999999999998</v>
+        <v>14.718</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>2.838000000000001</v>
+        <v>0.40600000000000058</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>55258</v>
+        <v>15394</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>55.258000000000003</v>
+        <v>15.394</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>0.13500000000000512</v>
+        <v>0.67600000000000016</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>55394</v>
+        <v>15799</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>55.393999999999998</v>
+        <v>15.798999999999999</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>0.13599999999999568</v>
+        <v>0.40499999999999936</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>56340</v>
+        <v>17015</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>56.34</v>
+        <v>17.015000000000001</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>0.94600000000000506</v>
+        <v>1.2160000000000011</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>56610</v>
+        <v>17421</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>56.61</v>
+        <v>17.420999999999999</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>0.26999999999999602</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>57015</v>
+        <v>17826</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>57.015000000000001</v>
+        <v>17.826000000000001</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
@@ -1491,7 +1478,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>57961</v>
+        <v>18231</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
@@ -1501,26 +1488,26 @@
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>57.960999999999999</v>
+        <v>18.231000000000002</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>0.94599999999999795</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>58367</v>
+        <v>18637</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>58.366999999999997</v>
+        <v>18.637</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
@@ -1529,45 +1516,45 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>59177</v>
+        <v>19042</v>
       </c>
       <c r="B35" t="s">
         <v>0</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>59.177</v>
+        <v>19.042000000000002</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
-        <v>0.81000000000000227</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>59312</v>
+        <v>19448</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>59.311999999999998</v>
+        <v>19.448</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>0.13499999999999801</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>59448</v>
+        <v>20258</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
@@ -1577,73 +1564,73 @@
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>59.448</v>
+        <v>20.257999999999999</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>0.13600000000000279</v>
+        <v>0.80999999999999872</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>59853</v>
+        <v>20664</v>
       </c>
       <c r="B38" t="s">
         <v>0</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>59.853000000000002</v>
+        <v>20.664000000000001</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <v>0.40600000000000236</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>59988</v>
+        <v>21069</v>
       </c>
       <c r="B39" t="s">
         <v>0</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>59.988</v>
+        <v>21.068999999999999</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
-        <v>0.13499999999999801</v>
+        <v>0.40499999999999758</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>60394</v>
+        <v>21475</v>
       </c>
       <c r="B40" t="s">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>60.393999999999998</v>
+        <v>21.475000000000001</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
-        <v>0.40599999999999881</v>
+        <v>0.40600000000000236</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>60529</v>
+        <v>21880</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
@@ -1653,168 +1640,168 @@
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>60.529000000000003</v>
+        <v>21.88</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
-        <v>0.13500000000000512</v>
+        <v>0.40499999999999758</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>60664</v>
+        <v>22285</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>60.664000000000001</v>
+        <v>22.285</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
-        <v>0.13499999999999801</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>61610</v>
+        <v>22691</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>61.61</v>
+        <v>22.690999999999999</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
-        <v>0.94599999999999795</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>61745</v>
+        <v>23502</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>61.744999999999997</v>
+        <v>23.501999999999999</v>
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
-        <v>0.13499999999999801</v>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>61880</v>
+        <v>23907</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>61.88</v>
+        <v>23.907</v>
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
-        <v>0.13500000000000512</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>62826</v>
+        <v>24312</v>
       </c>
       <c r="B46" t="s">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>62.826000000000001</v>
+        <v>24.312000000000001</v>
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
-        <v>0.94599999999999795</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>63096</v>
+        <v>24718</v>
       </c>
       <c r="B47" t="s">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>63.095999999999997</v>
+        <v>24.718</v>
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
-        <v>0.26999999999999602</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>63502</v>
+        <v>25123</v>
       </c>
       <c r="B48" t="s">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>63.502000000000002</v>
+        <v>25.123000000000001</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
-        <v>0.40600000000000591</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>64448</v>
+        <v>25529</v>
       </c>
       <c r="B49" t="s">
         <v>0</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>64.447999999999993</v>
+        <v>25.529</v>
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
-        <v>0.94599999999999085</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>64853</v>
+        <v>25934</v>
       </c>
       <c r="B50" t="s">
         <v>0</v>
@@ -1823,8 +1810,8 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <f t="shared" si="0"/>
-        <v>64.852999999999994</v>
+        <f>A50/1000</f>
+        <v>25.934000000000001</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
@@ -1833,121 +1820,121 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>64988</v>
+        <v>26745</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51">
-        <f t="shared" si="0"/>
-        <v>64.988</v>
+        <f t="shared" ref="D51:D114" si="2">A51/1000</f>
+        <v>26.745000000000001</v>
       </c>
       <c r="E51">
-        <f t="shared" si="1"/>
-        <v>0.13500000000000512</v>
+        <f>D51-D50</f>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>65123</v>
+        <v>29177</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <f t="shared" si="0"/>
-        <v>65.123000000000005</v>
+        <f t="shared" si="2"/>
+        <v>29.177</v>
       </c>
       <c r="E52">
-        <f t="shared" si="1"/>
-        <v>0.13500000000000512</v>
+        <f t="shared" ref="E52:E115" si="3">D52-D51</f>
+        <v>2.4319999999999986</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>65664</v>
+        <v>29988</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <f t="shared" si="0"/>
-        <v>65.664000000000001</v>
+        <f t="shared" si="2"/>
+        <v>29.988</v>
       </c>
       <c r="E53">
-        <f t="shared" si="1"/>
-        <v>0.54099999999999682</v>
+        <f t="shared" si="3"/>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>66340</v>
+        <v>30799</v>
       </c>
       <c r="B54" t="s">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54">
-        <f t="shared" si="0"/>
-        <v>66.34</v>
+        <f t="shared" si="2"/>
+        <v>30.798999999999999</v>
       </c>
       <c r="E54">
-        <f t="shared" si="1"/>
-        <v>0.67600000000000193</v>
+        <f t="shared" si="3"/>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>66475</v>
+        <v>31475</v>
       </c>
       <c r="B55" t="s">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <f t="shared" si="0"/>
-        <v>66.474999999999994</v>
+        <f t="shared" si="2"/>
+        <v>31.475000000000001</v>
       </c>
       <c r="E55">
-        <f t="shared" si="1"/>
-        <v>0.13499999999999091</v>
+        <f t="shared" si="3"/>
+        <v>0.67600000000000193</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>66880</v>
+        <v>32421</v>
       </c>
       <c r="B56" t="s">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56">
-        <f t="shared" si="0"/>
-        <v>66.88</v>
+        <f t="shared" si="2"/>
+        <v>32.420999999999999</v>
       </c>
       <c r="E56">
-        <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <f t="shared" si="3"/>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>67150</v>
+        <v>33907</v>
       </c>
       <c r="B57" t="s">
         <v>0</v>
@@ -1956,17 +1943,17 @@
         <v>2</v>
       </c>
       <c r="D57">
-        <f t="shared" si="0"/>
-        <v>67.150000000000006</v>
+        <f t="shared" si="2"/>
+        <v>33.906999999999996</v>
       </c>
       <c r="E57">
-        <f t="shared" si="1"/>
-        <v>0.27000000000001023</v>
+        <f t="shared" si="3"/>
+        <v>1.4859999999999971</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>68096</v>
+        <v>35664</v>
       </c>
       <c r="B58" t="s">
         <v>0</v>
@@ -1975,150 +1962,150 @@
         <v>0</v>
       </c>
       <c r="D58">
-        <f t="shared" si="0"/>
-        <v>68.096000000000004</v>
+        <f t="shared" si="2"/>
+        <v>35.664000000000001</v>
       </c>
       <c r="E58">
-        <f t="shared" si="1"/>
-        <v>0.94599999999999795</v>
+        <f t="shared" si="3"/>
+        <v>1.757000000000005</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>68231</v>
+        <v>36475</v>
       </c>
       <c r="B59" t="s">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <f t="shared" si="0"/>
-        <v>68.230999999999995</v>
+        <f t="shared" si="2"/>
+        <v>36.475000000000001</v>
       </c>
       <c r="E59">
-        <f t="shared" si="1"/>
-        <v>0.13499999999999091</v>
+        <f t="shared" si="3"/>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>68367</v>
+        <v>40529</v>
       </c>
       <c r="B60" t="s">
         <v>0</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60">
-        <f t="shared" si="0"/>
-        <v>68.367000000000004</v>
+        <f t="shared" si="2"/>
+        <v>40.529000000000003</v>
       </c>
       <c r="E60">
-        <f t="shared" si="1"/>
-        <v>0.13600000000000989</v>
+        <f t="shared" si="3"/>
+        <v>4.054000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>69312</v>
+        <v>42015</v>
       </c>
       <c r="B61" t="s">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <f t="shared" si="0"/>
-        <v>69.311999999999998</v>
+        <f t="shared" si="2"/>
+        <v>42.015000000000001</v>
       </c>
       <c r="E61">
-        <f t="shared" si="1"/>
-        <v>0.94499999999999318</v>
+        <f t="shared" si="3"/>
+        <v>1.4859999999999971</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>69583</v>
+        <v>42150</v>
       </c>
       <c r="B62" t="s">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <f t="shared" si="0"/>
-        <v>69.582999999999998</v>
+        <f t="shared" si="2"/>
+        <v>42.15</v>
       </c>
       <c r="E62">
-        <f t="shared" si="1"/>
-        <v>0.2710000000000008</v>
+        <f t="shared" si="3"/>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>69988</v>
+        <v>43772</v>
       </c>
       <c r="B63" t="s">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63">
-        <f t="shared" si="0"/>
-        <v>69.988</v>
+        <f t="shared" si="2"/>
+        <v>43.771999999999998</v>
       </c>
       <c r="E63">
-        <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <f t="shared" si="3"/>
+        <v>1.6219999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>70934</v>
+        <v>44448</v>
       </c>
       <c r="B64" t="s">
         <v>0</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <f t="shared" si="0"/>
-        <v>70.933999999999997</v>
+        <f t="shared" si="2"/>
+        <v>44.448</v>
       </c>
       <c r="E64">
-        <f t="shared" si="1"/>
-        <v>0.94599999999999795</v>
+        <f t="shared" si="3"/>
+        <v>0.67600000000000193</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>71340</v>
+        <v>45258</v>
       </c>
       <c r="B65" t="s">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <f t="shared" si="0"/>
-        <v>71.34</v>
+        <f t="shared" si="2"/>
+        <v>45.258000000000003</v>
       </c>
       <c r="E65">
-        <f t="shared" si="1"/>
-        <v>0.40600000000000591</v>
+        <f t="shared" si="3"/>
+        <v>0.81000000000000227</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>72015</v>
+        <v>45394</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
@@ -2127,169 +2114,169 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D116" si="2">A66/1000</f>
-        <v>72.015000000000001</v>
+        <f t="shared" si="2"/>
+        <v>45.393999999999998</v>
       </c>
       <c r="E66">
-        <f t="shared" si="1"/>
-        <v>0.67499999999999716</v>
+        <f t="shared" si="3"/>
+        <v>0.13599999999999568</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>72826</v>
+        <v>46204</v>
       </c>
       <c r="B67" t="s">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67">
         <f t="shared" si="2"/>
-        <v>72.825999999999993</v>
+        <v>46.204000000000001</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E116" si="3">D67-D66</f>
-        <v>0.81099999999999284</v>
+        <f t="shared" si="3"/>
+        <v>0.81000000000000227</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>72961</v>
+        <v>46475</v>
       </c>
       <c r="B68" t="s">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <f t="shared" si="2"/>
-        <v>72.960999999999999</v>
+        <v>46.475000000000001</v>
       </c>
       <c r="E68">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.2710000000000008</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>73367</v>
+        <v>47015</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69">
         <f t="shared" si="2"/>
-        <v>73.367000000000004</v>
+        <v>47.015000000000001</v>
       </c>
       <c r="E69">
         <f t="shared" si="3"/>
-        <v>0.40600000000000591</v>
+        <v>0.53999999999999915</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>73502</v>
+        <v>48502</v>
       </c>
       <c r="B70" t="s">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70">
         <f t="shared" si="2"/>
-        <v>73.501999999999995</v>
+        <v>48.502000000000002</v>
       </c>
       <c r="E70">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>1.4870000000000019</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>73637</v>
+        <v>48637</v>
       </c>
       <c r="B71" t="s">
         <v>0</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <f t="shared" si="2"/>
-        <v>73.637</v>
+        <v>48.637</v>
       </c>
       <c r="E71">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>74583</v>
+        <v>50258</v>
       </c>
       <c r="B72" t="s">
         <v>0</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D72">
         <f t="shared" si="2"/>
-        <v>74.582999999999998</v>
+        <v>50.258000000000003</v>
       </c>
       <c r="E72">
         <f t="shared" si="3"/>
-        <v>0.94599999999999795</v>
+        <v>1.6210000000000022</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>74718</v>
+        <v>50934</v>
       </c>
       <c r="B73" t="s">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <f t="shared" si="2"/>
-        <v>74.718000000000004</v>
+        <v>50.933999999999997</v>
       </c>
       <c r="E73">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.67599999999999483</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>74853</v>
+        <v>51880</v>
       </c>
       <c r="B74" t="s">
         <v>0</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D74">
         <f t="shared" si="2"/>
-        <v>74.852999999999994</v>
+        <v>51.88</v>
       </c>
       <c r="E74">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.94600000000000506</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>75394</v>
+        <v>52285</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
@@ -2299,16 +2286,16 @@
       </c>
       <c r="D75">
         <f t="shared" si="2"/>
-        <v>75.394000000000005</v>
+        <v>52.284999999999997</v>
       </c>
       <c r="E75">
         <f t="shared" si="3"/>
-        <v>0.54100000000001103</v>
+        <v>0.40499999999999403</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>76204</v>
+        <v>55123</v>
       </c>
       <c r="B76" t="s">
         <v>0</v>
@@ -2318,16 +2305,16 @@
       </c>
       <c r="D76">
         <f t="shared" si="2"/>
-        <v>76.203999999999994</v>
+        <v>55.122999999999998</v>
       </c>
       <c r="E76">
         <f t="shared" si="3"/>
-        <v>0.80999999999998806</v>
+        <v>2.838000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>76340</v>
+        <v>55258</v>
       </c>
       <c r="B77" t="s">
         <v>0</v>
@@ -2337,16 +2324,16 @@
       </c>
       <c r="D77">
         <f t="shared" si="2"/>
-        <v>76.34</v>
+        <v>55.258000000000003</v>
       </c>
       <c r="E77">
         <f t="shared" si="3"/>
-        <v>0.13600000000000989</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>76475</v>
+        <v>55394</v>
       </c>
       <c r="B78" t="s">
         <v>0</v>
@@ -2356,35 +2343,35 @@
       </c>
       <c r="D78">
         <f t="shared" si="2"/>
-        <v>76.474999999999994</v>
+        <v>55.393999999999998</v>
       </c>
       <c r="E78">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.13599999999999568</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>77015</v>
+        <v>56340</v>
       </c>
       <c r="B79" t="s">
         <v>0</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79">
         <f t="shared" si="2"/>
-        <v>77.015000000000001</v>
+        <v>56.34</v>
       </c>
       <c r="E79">
         <f t="shared" si="3"/>
-        <v>0.54000000000000625</v>
+        <v>0.94600000000000506</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>77826</v>
+        <v>56610</v>
       </c>
       <c r="B80" t="s">
         <v>0</v>
@@ -2394,16 +2381,16 @@
       </c>
       <c r="D80">
         <f t="shared" si="2"/>
-        <v>77.825999999999993</v>
+        <v>56.61</v>
       </c>
       <c r="E80">
         <f t="shared" si="3"/>
-        <v>0.81099999999999284</v>
+        <v>0.26999999999999602</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>77961</v>
+        <v>57015</v>
       </c>
       <c r="B81" t="s">
         <v>0</v>
@@ -2413,54 +2400,54 @@
       </c>
       <c r="D81">
         <f t="shared" si="2"/>
-        <v>77.960999999999999</v>
+        <v>57.015000000000001</v>
       </c>
       <c r="E81">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>78096</v>
+        <v>57961</v>
       </c>
       <c r="B82" t="s">
         <v>0</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D82">
         <f t="shared" si="2"/>
-        <v>78.096000000000004</v>
+        <v>57.960999999999999</v>
       </c>
       <c r="E82">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>78637</v>
+        <v>58367</v>
       </c>
       <c r="B83" t="s">
         <v>0</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83">
         <f t="shared" si="2"/>
-        <v>78.637</v>
+        <v>58.366999999999997</v>
       </c>
       <c r="E83">
         <f t="shared" si="3"/>
-        <v>0.54099999999999682</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>78907</v>
+        <v>59177</v>
       </c>
       <c r="B84" t="s">
         <v>0</v>
@@ -2470,111 +2457,111 @@
       </c>
       <c r="D84">
         <f t="shared" si="2"/>
-        <v>78.906999999999996</v>
+        <v>59.177</v>
       </c>
       <c r="E84">
         <f t="shared" si="3"/>
-        <v>0.26999999999999602</v>
+        <v>0.81000000000000227</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>79312</v>
+        <v>59312</v>
       </c>
       <c r="B85" t="s">
         <v>0</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85">
         <f t="shared" si="2"/>
-        <v>79.311999999999998</v>
+        <v>59.311999999999998</v>
       </c>
       <c r="E85">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>79448</v>
+        <v>59448</v>
       </c>
       <c r="B86" t="s">
         <v>0</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86">
         <f t="shared" si="2"/>
-        <v>79.447999999999993</v>
+        <v>59.448</v>
       </c>
       <c r="E86">
         <f t="shared" si="3"/>
-        <v>0.13599999999999568</v>
+        <v>0.13600000000000279</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>81069</v>
+        <v>59853</v>
       </c>
       <c r="B87" t="s">
         <v>0</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87">
         <f t="shared" si="2"/>
-        <v>81.069000000000003</v>
+        <v>59.853000000000002</v>
       </c>
       <c r="E87">
         <f t="shared" si="3"/>
-        <v>1.6210000000000093</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>81204</v>
+        <v>59988</v>
       </c>
       <c r="B88" t="s">
         <v>0</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D88">
         <f t="shared" si="2"/>
-        <v>81.203999999999994</v>
+        <v>59.988</v>
       </c>
       <c r="E88">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>81340</v>
+        <v>60394</v>
       </c>
       <c r="B89" t="s">
         <v>0</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89">
         <f t="shared" si="2"/>
-        <v>81.34</v>
+        <v>60.393999999999998</v>
       </c>
       <c r="E89">
         <f t="shared" si="3"/>
-        <v>0.13600000000000989</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>81880</v>
+        <v>60529</v>
       </c>
       <c r="B90" t="s">
         <v>0</v>
@@ -2584,16 +2571,16 @@
       </c>
       <c r="D90">
         <f t="shared" si="2"/>
-        <v>81.88</v>
+        <v>60.529000000000003</v>
       </c>
       <c r="E90">
         <f t="shared" si="3"/>
-        <v>0.53999999999999204</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>82015</v>
+        <v>60664</v>
       </c>
       <c r="B91" t="s">
         <v>0</v>
@@ -2603,35 +2590,35 @@
       </c>
       <c r="D91">
         <f t="shared" si="2"/>
-        <v>82.015000000000001</v>
+        <v>60.664000000000001</v>
       </c>
       <c r="E91">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>82150</v>
+        <v>61610</v>
       </c>
       <c r="B92" t="s">
         <v>0</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92">
         <f t="shared" si="2"/>
-        <v>82.15</v>
+        <v>61.61</v>
       </c>
       <c r="E92">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>82691</v>
+        <v>61745</v>
       </c>
       <c r="B93" t="s">
         <v>0</v>
@@ -2641,16 +2628,16 @@
       </c>
       <c r="D93">
         <f t="shared" si="2"/>
-        <v>82.691000000000003</v>
+        <v>61.744999999999997</v>
       </c>
       <c r="E93">
         <f t="shared" si="3"/>
-        <v>0.54099999999999682</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>82826</v>
+        <v>61880</v>
       </c>
       <c r="B94" t="s">
         <v>0</v>
@@ -2660,35 +2647,35 @@
       </c>
       <c r="D94">
         <f t="shared" si="2"/>
-        <v>82.825999999999993</v>
+        <v>61.88</v>
       </c>
       <c r="E94">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>82961</v>
+        <v>62826</v>
       </c>
       <c r="B95" t="s">
         <v>0</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D95">
         <f t="shared" si="2"/>
-        <v>82.960999999999999</v>
+        <v>62.826000000000001</v>
       </c>
       <c r="E95">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>83772</v>
+        <v>63096</v>
       </c>
       <c r="B96" t="s">
         <v>0</v>
@@ -2698,159 +2685,159 @@
       </c>
       <c r="D96">
         <f t="shared" si="2"/>
-        <v>83.772000000000006</v>
+        <v>63.095999999999997</v>
       </c>
       <c r="E96">
         <f t="shared" si="3"/>
-        <v>0.81100000000000705</v>
+        <v>0.26999999999999602</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>83907</v>
+        <v>63502</v>
       </c>
       <c r="B97" t="s">
         <v>0</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97">
         <f t="shared" si="2"/>
-        <v>83.906999999999996</v>
+        <v>63.502000000000002</v>
       </c>
       <c r="E97">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.40600000000000591</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>84312</v>
+        <v>64448</v>
       </c>
       <c r="B98" t="s">
         <v>0</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D98">
         <f t="shared" si="2"/>
-        <v>84.311999999999998</v>
+        <v>64.447999999999993</v>
       </c>
       <c r="E98">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>0.94599999999999085</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>85123</v>
+        <v>64853</v>
       </c>
       <c r="B99" t="s">
         <v>0</v>
       </c>
       <c r="C99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D99">
         <f t="shared" si="2"/>
-        <v>85.123000000000005</v>
+        <v>64.852999999999994</v>
       </c>
       <c r="E99">
         <f t="shared" si="3"/>
-        <v>0.81100000000000705</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>85934</v>
+        <v>64988</v>
       </c>
       <c r="B100" t="s">
         <v>0</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100">
         <f t="shared" si="2"/>
-        <v>85.933999999999997</v>
+        <v>64.988</v>
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
-        <v>0.81099999999999284</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>86204</v>
+        <v>65123</v>
       </c>
       <c r="B101" t="s">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101">
         <f t="shared" si="2"/>
-        <v>86.203999999999994</v>
+        <v>65.123000000000005</v>
       </c>
       <c r="E101">
         <f t="shared" si="3"/>
-        <v>0.26999999999999602</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>87556</v>
+        <v>65664</v>
       </c>
       <c r="B102" t="s">
         <v>0</v>
       </c>
       <c r="C102">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <f t="shared" si="2"/>
-        <v>87.555999999999997</v>
+        <v>65.664000000000001</v>
       </c>
       <c r="E102">
         <f t="shared" si="3"/>
-        <v>1.3520000000000039</v>
+        <v>0.54099999999999682</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>87691</v>
+        <v>66340</v>
       </c>
       <c r="B103" t="s">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D103">
         <f t="shared" si="2"/>
-        <v>87.691000000000003</v>
+        <v>66.34</v>
       </c>
       <c r="E103">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.67600000000000193</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>87826</v>
+        <v>66475</v>
       </c>
       <c r="B104" t="s">
         <v>0</v>
       </c>
       <c r="C104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D104">
         <f t="shared" si="2"/>
-        <v>87.825999999999993</v>
+        <v>66.474999999999994</v>
       </c>
       <c r="E104">
         <f t="shared" si="3"/>
@@ -2859,102 +2846,102 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>88772</v>
+        <v>66880</v>
       </c>
       <c r="B105" t="s">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D105">
         <f t="shared" si="2"/>
-        <v>88.772000000000006</v>
+        <v>66.88</v>
       </c>
       <c r="E105">
         <f t="shared" si="3"/>
-        <v>0.94600000000001216</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>89042</v>
+        <v>67150</v>
       </c>
       <c r="B106" t="s">
         <v>0</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D106">
         <f t="shared" si="2"/>
-        <v>89.042000000000002</v>
+        <v>67.150000000000006</v>
       </c>
       <c r="E106">
         <f t="shared" si="3"/>
-        <v>0.26999999999999602</v>
+        <v>0.27000000000001023</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>89448</v>
+        <v>68096</v>
       </c>
       <c r="B107" t="s">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107">
         <f t="shared" si="2"/>
-        <v>89.447999999999993</v>
+        <v>68.096000000000004</v>
       </c>
       <c r="E107">
         <f t="shared" si="3"/>
-        <v>0.4059999999999917</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>90394</v>
+        <v>68231</v>
       </c>
       <c r="B108" t="s">
         <v>0</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D108">
         <f t="shared" si="2"/>
-        <v>90.394000000000005</v>
+        <v>68.230999999999995</v>
       </c>
       <c r="E108">
         <f t="shared" si="3"/>
-        <v>0.94600000000001216</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>90529</v>
+        <v>68367</v>
       </c>
       <c r="B109" t="s">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D109">
         <f t="shared" si="2"/>
-        <v>90.528999999999996</v>
+        <v>68.367000000000004</v>
       </c>
       <c r="E109">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.13600000000000989</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>90664</v>
+        <v>69312</v>
       </c>
       <c r="B110" t="s">
         <v>0</v>
@@ -2964,16 +2951,16 @@
       </c>
       <c r="D110">
         <f t="shared" si="2"/>
-        <v>90.664000000000001</v>
+        <v>69.311999999999998</v>
       </c>
       <c r="E110">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.94499999999999318</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>90799</v>
+        <v>69583</v>
       </c>
       <c r="B111" t="s">
         <v>0</v>
@@ -2983,35 +2970,35 @@
       </c>
       <c r="D111">
         <f t="shared" si="2"/>
-        <v>90.799000000000007</v>
+        <v>69.582999999999998</v>
       </c>
       <c r="E111">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.2710000000000008</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>91610</v>
+        <v>69988</v>
       </c>
       <c r="B112" t="s">
         <v>0</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D112">
         <f t="shared" si="2"/>
-        <v>91.61</v>
+        <v>69.988</v>
       </c>
       <c r="E112">
         <f t="shared" si="3"/>
-        <v>0.81099999999999284</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>91745</v>
+        <v>70934</v>
       </c>
       <c r="B113" t="s">
         <v>0</v>
@@ -3021,67 +3008,998 @@
       </c>
       <c r="D113">
         <f t="shared" si="2"/>
-        <v>91.745000000000005</v>
+        <v>70.933999999999997</v>
       </c>
       <c r="E113">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>91880</v>
+        <v>71340</v>
       </c>
       <c r="B114" t="s">
         <v>0</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D114">
         <f t="shared" si="2"/>
-        <v>91.88</v>
+        <v>71.34</v>
       </c>
       <c r="E114">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.40600000000000591</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>92285</v>
+        <v>72015</v>
       </c>
       <c r="B115" t="s">
         <v>0</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <f t="shared" si="2"/>
-        <v>92.284999999999997</v>
+        <f t="shared" ref="D115:D165" si="4">A115/1000</f>
+        <v>72.015000000000001</v>
       </c>
       <c r="E115">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>0.67499999999999716</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
+        <v>72826</v>
+      </c>
+      <c r="B116" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="4"/>
+        <v>72.825999999999993</v>
+      </c>
+      <c r="E116">
+        <f t="shared" ref="E116:E165" si="5">D116-D115</f>
+        <v>0.81099999999999284</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>72961</v>
+      </c>
+      <c r="B117" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="4"/>
+        <v>72.960999999999999</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>73367</v>
+      </c>
+      <c r="B118" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="4"/>
+        <v>73.367000000000004</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="5"/>
+        <v>0.40600000000000591</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>73502</v>
+      </c>
+      <c r="B119" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="4"/>
+        <v>73.501999999999995</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>73637</v>
+      </c>
+      <c r="B120" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="4"/>
+        <v>73.637</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>74583</v>
+      </c>
+      <c r="B121" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="4"/>
+        <v>74.582999999999998</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="5"/>
+        <v>0.94599999999999795</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>74718</v>
+      </c>
+      <c r="B122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="4"/>
+        <v>74.718000000000004</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>74853</v>
+      </c>
+      <c r="B123" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="4"/>
+        <v>74.852999999999994</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>75394</v>
+      </c>
+      <c r="B124" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="4"/>
+        <v>75.394000000000005</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="5"/>
+        <v>0.54100000000001103</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>76204</v>
+      </c>
+      <c r="B125" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="4"/>
+        <v>76.203999999999994</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="5"/>
+        <v>0.80999999999998806</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>76340</v>
+      </c>
+      <c r="B126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="4"/>
+        <v>76.34</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="5"/>
+        <v>0.13600000000000989</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>76475</v>
+      </c>
+      <c r="B127" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="4"/>
+        <v>76.474999999999994</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>77015</v>
+      </c>
+      <c r="B128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="4"/>
+        <v>77.015000000000001</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="5"/>
+        <v>0.54000000000000625</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>77826</v>
+      </c>
+      <c r="B129" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="4"/>
+        <v>77.825999999999993</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="5"/>
+        <v>0.81099999999999284</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>77961</v>
+      </c>
+      <c r="B130" t="s">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="4"/>
+        <v>77.960999999999999</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>78096</v>
+      </c>
+      <c r="B131" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="4"/>
+        <v>78.096000000000004</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>78637</v>
+      </c>
+      <c r="B132" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="4"/>
+        <v>78.637</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="5"/>
+        <v>0.54099999999999682</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>78907</v>
+      </c>
+      <c r="B133" t="s">
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="4"/>
+        <v>78.906999999999996</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="5"/>
+        <v>0.26999999999999602</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>79312</v>
+      </c>
+      <c r="B134" t="s">
+        <v>0</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="4"/>
+        <v>79.311999999999998</v>
+      </c>
+      <c r="E134">
+        <f t="shared" si="5"/>
+        <v>0.40500000000000114</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>79448</v>
+      </c>
+      <c r="B135" t="s">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="4"/>
+        <v>79.447999999999993</v>
+      </c>
+      <c r="E135">
+        <f t="shared" si="5"/>
+        <v>0.13599999999999568</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>81069</v>
+      </c>
+      <c r="B136" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="4"/>
+        <v>81.069000000000003</v>
+      </c>
+      <c r="E136">
+        <f t="shared" si="5"/>
+        <v>1.6210000000000093</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>81204</v>
+      </c>
+      <c r="B137" t="s">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="4"/>
+        <v>81.203999999999994</v>
+      </c>
+      <c r="E137">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>81340</v>
+      </c>
+      <c r="B138" t="s">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138">
+        <f t="shared" si="4"/>
+        <v>81.34</v>
+      </c>
+      <c r="E138">
+        <f t="shared" si="5"/>
+        <v>0.13600000000000989</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>81880</v>
+      </c>
+      <c r="B139" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="4"/>
+        <v>81.88</v>
+      </c>
+      <c r="E139">
+        <f t="shared" si="5"/>
+        <v>0.53999999999999204</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>82015</v>
+      </c>
+      <c r="B140" t="s">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="4"/>
+        <v>82.015000000000001</v>
+      </c>
+      <c r="E140">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>82150</v>
+      </c>
+      <c r="B141" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <f t="shared" si="4"/>
+        <v>82.15</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>82691</v>
+      </c>
+      <c r="B142" t="s">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="4"/>
+        <v>82.691000000000003</v>
+      </c>
+      <c r="E142">
+        <f t="shared" si="5"/>
+        <v>0.54099999999999682</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>82826</v>
+      </c>
+      <c r="B143" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="4"/>
+        <v>82.825999999999993</v>
+      </c>
+      <c r="E143">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>82961</v>
+      </c>
+      <c r="B144" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="4"/>
+        <v>82.960999999999999</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>83772</v>
+      </c>
+      <c r="B145" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="4"/>
+        <v>83.772000000000006</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="5"/>
+        <v>0.81100000000000705</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>83907</v>
+      </c>
+      <c r="B146" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>2</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="4"/>
+        <v>83.906999999999996</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>84312</v>
+      </c>
+      <c r="B147" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="4"/>
+        <v>84.311999999999998</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="5"/>
+        <v>0.40500000000000114</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>85123</v>
+      </c>
+      <c r="B148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="4"/>
+        <v>85.123000000000005</v>
+      </c>
+      <c r="E148">
+        <f t="shared" si="5"/>
+        <v>0.81100000000000705</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>85934</v>
+      </c>
+      <c r="B149" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="4"/>
+        <v>85.933999999999997</v>
+      </c>
+      <c r="E149">
+        <f t="shared" si="5"/>
+        <v>0.81099999999999284</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>86204</v>
+      </c>
+      <c r="B150" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="4"/>
+        <v>86.203999999999994</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="5"/>
+        <v>0.26999999999999602</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>87556</v>
+      </c>
+      <c r="B151" t="s">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>2</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="4"/>
+        <v>87.555999999999997</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="5"/>
+        <v>1.3520000000000039</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>87691</v>
+      </c>
+      <c r="B152" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>2</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="4"/>
+        <v>87.691000000000003</v>
+      </c>
+      <c r="E152">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>87826</v>
+      </c>
+      <c r="B153" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153">
+        <f t="shared" si="4"/>
+        <v>87.825999999999993</v>
+      </c>
+      <c r="E153">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>88772</v>
+      </c>
+      <c r="B154" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <f t="shared" si="4"/>
+        <v>88.772000000000006</v>
+      </c>
+      <c r="E154">
+        <f t="shared" si="5"/>
+        <v>0.94600000000001216</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>89042</v>
+      </c>
+      <c r="B155" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <f t="shared" si="4"/>
+        <v>89.042000000000002</v>
+      </c>
+      <c r="E155">
+        <f t="shared" si="5"/>
+        <v>0.26999999999999602</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>89448</v>
+      </c>
+      <c r="B156" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <f t="shared" si="4"/>
+        <v>89.447999999999993</v>
+      </c>
+      <c r="E156">
+        <f t="shared" si="5"/>
+        <v>0.4059999999999917</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>90394</v>
+      </c>
+      <c r="B157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>2</v>
+      </c>
+      <c r="D157">
+        <f t="shared" si="4"/>
+        <v>90.394000000000005</v>
+      </c>
+      <c r="E157">
+        <f t="shared" si="5"/>
+        <v>0.94600000000001216</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>90529</v>
+      </c>
+      <c r="B158" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>2</v>
+      </c>
+      <c r="D158">
+        <f t="shared" si="4"/>
+        <v>90.528999999999996</v>
+      </c>
+      <c r="E158">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>90664</v>
+      </c>
+      <c r="B159" t="s">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>2</v>
+      </c>
+      <c r="D159">
+        <f t="shared" si="4"/>
+        <v>90.664000000000001</v>
+      </c>
+      <c r="E159">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>90799</v>
+      </c>
+      <c r="B160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>2</v>
+      </c>
+      <c r="D160">
+        <f t="shared" si="4"/>
+        <v>90.799000000000007</v>
+      </c>
+      <c r="E160">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>91610</v>
+      </c>
+      <c r="B161" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <f t="shared" si="4"/>
+        <v>91.61</v>
+      </c>
+      <c r="E161">
+        <f t="shared" si="5"/>
+        <v>0.81099999999999284</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>91745</v>
+      </c>
+      <c r="B162" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <f t="shared" si="4"/>
+        <v>91.745000000000005</v>
+      </c>
+      <c r="E162">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>91880</v>
+      </c>
+      <c r="B163" t="s">
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <f t="shared" si="4"/>
+        <v>91.88</v>
+      </c>
+      <c r="E163">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>92285</v>
+      </c>
+      <c r="B164" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <f t="shared" si="4"/>
+        <v>92.284999999999997</v>
+      </c>
+      <c r="E164">
+        <f t="shared" si="5"/>
+        <v>0.40500000000000114</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165">
         <v>92421</v>
       </c>
-      <c r="B116" t="s">
-        <v>0</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-      <c r="D116">
-        <f t="shared" si="2"/>
+      <c r="B165" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+      <c r="D165">
+        <f t="shared" si="4"/>
         <v>92.421000000000006</v>
       </c>
-      <c r="E116">
-        <f t="shared" si="3"/>
+      <c r="E165">
+        <f t="shared" si="5"/>
         <v>0.13600000000000989</v>
       </c>
     </row>

</xml_diff>

<commit_message>
temp change time shows instead of accuracy
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dead to Me/deadtome.xlsx
+++ b/Assets/Resources/Dead to Me/deadtome.xlsx
@@ -5,18 +5,31 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rhythm-Road\Rhythm-Road\Assets\Resources\Dead to Me\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\College\Software - Project 2 COMP313\Rhythm-Road\Assets\Resources\Dead to Me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0065BE8-F1A6-414B-9FC7-0A16F919D41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390B85A6-029C-4002-A558-C34F8639A9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17955" yWindow="3585" windowWidth="21600" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="greatdays" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -866,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:C165"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
dead to me obstacles added
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dead to Me/deadtome.xlsx
+++ b/Assets/Resources/Dead to Me/deadtome.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\College\Software - Project 2 COMP313\Rhythm-Road\Assets\Resources\Dead to Me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390B85A6-029C-4002-A558-C34F8639A9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59EF5A3-5D0B-4E99-B9B7-736259CFF5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17955" yWindow="3585" windowWidth="21600" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="greatdays" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="4">
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -877,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <f t="shared" ref="D1:D49" si="0">A1/1000</f>
+        <f t="shared" ref="D1:D51" si="0">A1/1000</f>
         <v>2.0150000000000001</v>
       </c>
     </row>
@@ -915,7 +924,7 @@
         <v>2.4209999999999998</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E50" si="1">D2-D1</f>
+        <f t="shared" ref="E2:E52" si="1">D2-D1</f>
         <v>0.40599999999999969</v>
       </c>
     </row>
@@ -1342,10 +1351,10 @@
         <v>13907</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -1358,140 +1367,140 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>14312</v>
+        <v>13907</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>14.311999999999999</v>
+        <v>13.907</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>0.40499999999999936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>14718</v>
+        <v>13907</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>14.718</v>
+        <v>13.907</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>0.40600000000000058</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>15394</v>
+        <v>14312</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>15.394</v>
+        <v>14.311999999999999</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>0.67600000000000016</v>
+        <v>0.40499999999999936</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>15799</v>
+        <v>14718</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>15.798999999999999</v>
+        <v>14.718</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>0.40499999999999936</v>
+        <v>0.40600000000000058</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>17015</v>
+        <v>15394</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>17.015000000000001</v>
+        <v>15.394</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>1.2160000000000011</v>
+        <v>0.67600000000000016</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>17421</v>
+        <v>15799</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>17.420999999999999</v>
+        <v>15.798999999999999</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>0.40599999999999881</v>
+        <v>0.40499999999999936</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>17826</v>
+        <v>17015</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>17.826000000000001</v>
+        <v>17.015000000000001</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <v>1.2160000000000011</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>18231</v>
+        <v>17421</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
@@ -1501,16 +1510,16 @@
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>18.231000000000002</v>
+        <v>17.420999999999999</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>18637</v>
+        <v>17826</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
@@ -1520,16 +1529,16 @@
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>18.637</v>
+        <v>17.826000000000001</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>0.40599999999999881</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>19042</v>
+        <v>18231</v>
       </c>
       <c r="B35" t="s">
         <v>0</v>
@@ -1539,7 +1548,7 @@
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>19.042000000000002</v>
+        <v>18.231000000000002</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
@@ -1548,7 +1557,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>19448</v>
+        <v>18637</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
@@ -1558,7 +1567,7 @@
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>19.448</v>
+        <v>18.637</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
@@ -1567,74 +1576,74 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>20258</v>
+        <v>19042</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>20.257999999999999</v>
+        <v>19.042000000000002</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>0.80999999999999872</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>20664</v>
+        <v>19448</v>
       </c>
       <c r="B38" t="s">
         <v>0</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>20.664000000000001</v>
+        <v>19.448</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>0.40600000000000236</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>21069</v>
+        <v>20258</v>
       </c>
       <c r="B39" t="s">
         <v>0</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>21.068999999999999</v>
+        <v>20.257999999999999</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
-        <v>0.40499999999999758</v>
+        <v>0.80999999999999872</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>21475</v>
+        <v>20664</v>
       </c>
       <c r="B40" t="s">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>21.475000000000001</v>
+        <v>20.664000000000001</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
@@ -1643,7 +1652,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>21880</v>
+        <v>21069</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
@@ -1653,7 +1662,7 @@
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>21.88</v>
+        <v>21.068999999999999</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
@@ -1662,26 +1671,26 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>22285</v>
+        <v>21475</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>22.285</v>
+        <v>21.475000000000001</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <v>0.40600000000000236</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>22691</v>
+        <v>21880</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
@@ -1691,35 +1700,35 @@
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>22.690999999999999</v>
+        <v>21.88</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
-        <v>0.40599999999999881</v>
+        <v>0.40499999999999758</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>23502</v>
+        <v>22285</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>23.501999999999999</v>
+        <v>22.285</v>
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
-        <v>0.81099999999999994</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>23907</v>
+        <v>22691</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -1729,35 +1738,35 @@
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>23.907</v>
+        <v>22.690999999999999</v>
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>24312</v>
+        <v>23502</v>
       </c>
       <c r="B46" t="s">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>24.312000000000001</v>
+        <v>23.501999999999999</v>
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
-        <v>0.40500000000000114</v>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>24718</v>
+        <v>23907</v>
       </c>
       <c r="B47" t="s">
         <v>0</v>
@@ -1767,26 +1776,26 @@
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>24.718</v>
+        <v>23.907</v>
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
-        <v>0.40599999999999881</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>25123</v>
+        <v>24312</v>
       </c>
       <c r="B48" t="s">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>25.123000000000001</v>
+        <v>24.312000000000001</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
@@ -1795,7 +1804,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>25529</v>
+        <v>24718</v>
       </c>
       <c r="B49" t="s">
         <v>0</v>
@@ -1805,7 +1814,7 @@
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>25.529</v>
+        <v>24.718</v>
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
@@ -1814,17 +1823,17 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>25934</v>
+        <v>25123</v>
       </c>
       <c r="B50" t="s">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50">
-        <f>A50/1000</f>
-        <v>25.934000000000001</v>
+        <f t="shared" si="0"/>
+        <v>25.123000000000001</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
@@ -1833,254 +1842,254 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>26745</v>
+        <v>25529</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <f t="shared" ref="D51:D114" si="2">A51/1000</f>
-        <v>26.745000000000001</v>
+        <f t="shared" si="0"/>
+        <v>25.529</v>
       </c>
       <c r="E51">
-        <f>D51-D50</f>
-        <v>0.81099999999999994</v>
+        <f t="shared" si="1"/>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>29177</v>
+        <v>25934</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
-        <f t="shared" si="2"/>
-        <v>29.177</v>
+        <f>A52/1000</f>
+        <v>25.934000000000001</v>
       </c>
       <c r="E52">
-        <f t="shared" ref="E52:E115" si="3">D52-D51</f>
-        <v>2.4319999999999986</v>
+        <f t="shared" si="1"/>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>29988</v>
+        <v>26745</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53">
-        <f t="shared" si="2"/>
-        <v>29.988</v>
+        <f t="shared" ref="D53:D119" si="2">A53/1000</f>
+        <v>26.745000000000001</v>
       </c>
       <c r="E53">
-        <f t="shared" si="3"/>
+        <f>D53-D52</f>
         <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>30799</v>
+        <v>29177</v>
       </c>
       <c r="B54" t="s">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D54">
         <f t="shared" si="2"/>
-        <v>30.798999999999999</v>
+        <v>29.177</v>
       </c>
       <c r="E54">
-        <f t="shared" si="3"/>
-        <v>0.81099999999999994</v>
+        <f t="shared" ref="E54:E120" si="3">D54-D53</f>
+        <v>2.4319999999999986</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>31475</v>
+        <v>29988</v>
       </c>
       <c r="B55" t="s">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <f t="shared" si="2"/>
-        <v>31.475000000000001</v>
+        <v>29.988</v>
       </c>
       <c r="E55">
         <f t="shared" si="3"/>
-        <v>0.67600000000000193</v>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>32421</v>
+        <v>30394</v>
       </c>
       <c r="B56" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56">
         <f t="shared" si="2"/>
-        <v>32.420999999999999</v>
+        <v>30.393999999999998</v>
       </c>
       <c r="E56">
         <f t="shared" si="3"/>
-        <v>0.94599999999999795</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>33907</v>
+        <v>30394</v>
       </c>
       <c r="B57" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <f t="shared" si="2"/>
-        <v>33.906999999999996</v>
+        <v>30.393999999999998</v>
       </c>
       <c r="E57">
         <f t="shared" si="3"/>
-        <v>1.4859999999999971</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>35664</v>
+        <v>30394</v>
       </c>
       <c r="B58" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D58">
         <f t="shared" si="2"/>
-        <v>35.664000000000001</v>
+        <v>30.393999999999998</v>
       </c>
       <c r="E58">
         <f t="shared" si="3"/>
-        <v>1.757000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>36475</v>
+        <v>30799</v>
       </c>
       <c r="B59" t="s">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59">
         <f t="shared" si="2"/>
-        <v>36.475000000000001</v>
+        <v>30.798999999999999</v>
       </c>
       <c r="E59">
         <f t="shared" si="3"/>
-        <v>0.81099999999999994</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>40529</v>
+        <v>31475</v>
       </c>
       <c r="B60" t="s">
         <v>0</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D60">
         <f t="shared" si="2"/>
-        <v>40.529000000000003</v>
+        <v>31.475000000000001</v>
       </c>
       <c r="E60">
         <f t="shared" si="3"/>
-        <v>4.054000000000002</v>
+        <v>0.67600000000000193</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>42015</v>
+        <v>32421</v>
       </c>
       <c r="B61" t="s">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <f t="shared" si="2"/>
-        <v>42.015000000000001</v>
+        <v>32.420999999999999</v>
       </c>
       <c r="E61">
         <f t="shared" si="3"/>
-        <v>1.4859999999999971</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>42150</v>
+        <v>33907</v>
       </c>
       <c r="B62" t="s">
         <v>0</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62">
         <f t="shared" si="2"/>
-        <v>42.15</v>
+        <v>33.906999999999996</v>
       </c>
       <c r="E62">
         <f t="shared" si="3"/>
-        <v>0.13499999999999801</v>
+        <v>1.4859999999999971</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>43772</v>
+        <v>35664</v>
       </c>
       <c r="B63" t="s">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D63">
         <f t="shared" si="2"/>
-        <v>43.771999999999998</v>
+        <v>35.664000000000001</v>
       </c>
       <c r="E63">
         <f t="shared" si="3"/>
-        <v>1.6219999999999999</v>
+        <v>1.757000000000005</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>44448</v>
+        <v>36475</v>
       </c>
       <c r="B64" t="s">
         <v>0</v>
@@ -2090,35 +2099,35 @@
       </c>
       <c r="D64">
         <f t="shared" si="2"/>
-        <v>44.448</v>
+        <v>36.475000000000001</v>
       </c>
       <c r="E64">
         <f t="shared" si="3"/>
-        <v>0.67600000000000193</v>
+        <v>0.81099999999999994</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>45258</v>
+        <v>40529</v>
       </c>
       <c r="B65" t="s">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D65">
         <f t="shared" si="2"/>
-        <v>45.258000000000003</v>
+        <v>40.529000000000003</v>
       </c>
       <c r="E65">
         <f t="shared" si="3"/>
-        <v>0.81000000000000227</v>
+        <v>4.054000000000002</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>45394</v>
+        <v>42015</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
@@ -2128,73 +2137,73 @@
       </c>
       <c r="D66">
         <f t="shared" si="2"/>
-        <v>45.393999999999998</v>
+        <v>42.015000000000001</v>
       </c>
       <c r="E66">
         <f t="shared" si="3"/>
-        <v>0.13599999999999568</v>
+        <v>1.4859999999999971</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>46204</v>
+        <v>42150</v>
       </c>
       <c r="B67" t="s">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
         <f t="shared" si="2"/>
-        <v>46.204000000000001</v>
+        <v>42.15</v>
       </c>
       <c r="E67">
         <f t="shared" si="3"/>
-        <v>0.81000000000000227</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>46475</v>
+        <v>43772</v>
       </c>
       <c r="B68" t="s">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D68">
         <f t="shared" si="2"/>
-        <v>46.475000000000001</v>
+        <v>43.771999999999998</v>
       </c>
       <c r="E68">
         <f t="shared" si="3"/>
-        <v>0.2710000000000008</v>
+        <v>1.6219999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>47015</v>
+        <v>44448</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <f t="shared" si="2"/>
-        <v>47.015000000000001</v>
+        <v>44.448</v>
       </c>
       <c r="E69">
         <f t="shared" si="3"/>
-        <v>0.53999999999999915</v>
+        <v>0.67600000000000193</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>48502</v>
+        <v>45258</v>
       </c>
       <c r="B70" t="s">
         <v>0</v>
@@ -2204,16 +2213,16 @@
       </c>
       <c r="D70">
         <f t="shared" si="2"/>
-        <v>48.502000000000002</v>
+        <v>45.258000000000003</v>
       </c>
       <c r="E70">
         <f t="shared" si="3"/>
-        <v>1.4870000000000019</v>
+        <v>0.81000000000000227</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>48637</v>
+        <v>45394</v>
       </c>
       <c r="B71" t="s">
         <v>0</v>
@@ -2223,35 +2232,35 @@
       </c>
       <c r="D71">
         <f t="shared" si="2"/>
-        <v>48.637</v>
+        <v>45.393999999999998</v>
       </c>
       <c r="E71">
         <f t="shared" si="3"/>
-        <v>0.13499999999999801</v>
+        <v>0.13599999999999568</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>50258</v>
+        <v>46204</v>
       </c>
       <c r="B72" t="s">
         <v>0</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <f t="shared" si="2"/>
-        <v>50.258000000000003</v>
+        <v>46.204000000000001</v>
       </c>
       <c r="E72">
         <f t="shared" si="3"/>
-        <v>1.6210000000000022</v>
+        <v>0.81000000000000227</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>50934</v>
+        <v>46475</v>
       </c>
       <c r="B73" t="s">
         <v>0</v>
@@ -2261,16 +2270,16 @@
       </c>
       <c r="D73">
         <f t="shared" si="2"/>
-        <v>50.933999999999997</v>
+        <v>46.475000000000001</v>
       </c>
       <c r="E73">
         <f t="shared" si="3"/>
-        <v>0.67599999999999483</v>
+        <v>0.2710000000000008</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>51880</v>
+        <v>47015</v>
       </c>
       <c r="B74" t="s">
         <v>0</v>
@@ -2280,54 +2289,54 @@
       </c>
       <c r="D74">
         <f t="shared" si="2"/>
-        <v>51.88</v>
+        <v>47.015000000000001</v>
       </c>
       <c r="E74">
         <f t="shared" si="3"/>
-        <v>0.94600000000000506</v>
+        <v>0.53999999999999915</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>52285</v>
+        <v>48502</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75">
         <f t="shared" si="2"/>
-        <v>52.284999999999997</v>
+        <v>48.502000000000002</v>
       </c>
       <c r="E75">
         <f t="shared" si="3"/>
-        <v>0.40499999999999403</v>
+        <v>1.4870000000000019</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>55123</v>
+        <v>48637</v>
       </c>
       <c r="B76" t="s">
         <v>0</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D76">
         <f t="shared" si="2"/>
-        <v>55.122999999999998</v>
+        <v>48.637</v>
       </c>
       <c r="E76">
         <f t="shared" si="3"/>
-        <v>2.838000000000001</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>55258</v>
+        <v>50258</v>
       </c>
       <c r="B77" t="s">
         <v>0</v>
@@ -2337,45 +2346,45 @@
       </c>
       <c r="D77">
         <f t="shared" si="2"/>
-        <v>55.258000000000003</v>
+        <v>50.258000000000003</v>
       </c>
       <c r="E77">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>1.6210000000000022</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>55394</v>
+        <v>50934</v>
       </c>
       <c r="B78" t="s">
         <v>0</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <f t="shared" si="2"/>
-        <v>55.393999999999998</v>
+        <v>50.933999999999997</v>
       </c>
       <c r="E78">
         <f t="shared" si="3"/>
-        <v>0.13599999999999568</v>
+        <v>0.67599999999999483</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>56340</v>
+        <v>51880</v>
       </c>
       <c r="B79" t="s">
         <v>0</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79">
         <f t="shared" si="2"/>
-        <v>56.34</v>
+        <v>51.88</v>
       </c>
       <c r="E79">
         <f t="shared" si="3"/>
@@ -2384,45 +2393,45 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>56610</v>
+        <v>52285</v>
       </c>
       <c r="B80" t="s">
         <v>0</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <f t="shared" si="2"/>
-        <v>56.61</v>
+        <v>52.284999999999997</v>
       </c>
       <c r="E80">
         <f t="shared" si="3"/>
-        <v>0.26999999999999602</v>
+        <v>0.40499999999999403</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>57015</v>
+        <v>55123</v>
       </c>
       <c r="B81" t="s">
         <v>0</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D81">
         <f t="shared" si="2"/>
-        <v>57.015000000000001</v>
+        <v>55.122999999999998</v>
       </c>
       <c r="E81">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>2.838000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>57961</v>
+        <v>55258</v>
       </c>
       <c r="B82" t="s">
         <v>0</v>
@@ -2432,16 +2441,16 @@
       </c>
       <c r="D82">
         <f t="shared" si="2"/>
-        <v>57.960999999999999</v>
+        <v>55.258000000000003</v>
       </c>
       <c r="E82">
         <f t="shared" si="3"/>
-        <v>0.94599999999999795</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>58367</v>
+        <v>55394</v>
       </c>
       <c r="B83" t="s">
         <v>0</v>
@@ -2451,16 +2460,16 @@
       </c>
       <c r="D83">
         <f t="shared" si="2"/>
-        <v>58.366999999999997</v>
+        <v>55.393999999999998</v>
       </c>
       <c r="E83">
         <f t="shared" si="3"/>
-        <v>0.40599999999999881</v>
+        <v>0.13599999999999568</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>59177</v>
+        <v>56340</v>
       </c>
       <c r="B84" t="s">
         <v>0</v>
@@ -2470,16 +2479,16 @@
       </c>
       <c r="D84">
         <f t="shared" si="2"/>
-        <v>59.177</v>
+        <v>56.34</v>
       </c>
       <c r="E84">
         <f t="shared" si="3"/>
-        <v>0.81000000000000227</v>
+        <v>0.94600000000000506</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>59312</v>
+        <v>56610</v>
       </c>
       <c r="B85" t="s">
         <v>0</v>
@@ -2489,16 +2498,16 @@
       </c>
       <c r="D85">
         <f t="shared" si="2"/>
-        <v>59.311999999999998</v>
+        <v>56.61</v>
       </c>
       <c r="E85">
         <f t="shared" si="3"/>
-        <v>0.13499999999999801</v>
+        <v>0.26999999999999602</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>59448</v>
+        <v>57015</v>
       </c>
       <c r="B86" t="s">
         <v>0</v>
@@ -2508,130 +2517,130 @@
       </c>
       <c r="D86">
         <f t="shared" si="2"/>
-        <v>59.448</v>
+        <v>57.015000000000001</v>
       </c>
       <c r="E86">
         <f t="shared" si="3"/>
-        <v>0.13600000000000279</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>59853</v>
+        <v>57961</v>
       </c>
       <c r="B87" t="s">
         <v>0</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D87">
         <f t="shared" si="2"/>
-        <v>59.853000000000002</v>
+        <v>57.960999999999999</v>
       </c>
       <c r="E87">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>59988</v>
+        <v>58367</v>
       </c>
       <c r="B88" t="s">
         <v>0</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D88">
         <f t="shared" si="2"/>
-        <v>59.988</v>
+        <v>58.366999999999997</v>
       </c>
       <c r="E88">
         <f t="shared" si="3"/>
-        <v>0.13499999999999801</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>60394</v>
+        <v>59177</v>
       </c>
       <c r="B89" t="s">
         <v>0</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89">
         <f t="shared" si="2"/>
-        <v>60.393999999999998</v>
+        <v>59.177</v>
       </c>
       <c r="E89">
         <f t="shared" si="3"/>
-        <v>0.40599999999999881</v>
+        <v>0.81000000000000227</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>60529</v>
+        <v>59312</v>
       </c>
       <c r="B90" t="s">
         <v>0</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90">
         <f t="shared" si="2"/>
-        <v>60.529000000000003</v>
+        <v>59.311999999999998</v>
       </c>
       <c r="E90">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>60664</v>
+        <v>59448</v>
       </c>
       <c r="B91" t="s">
         <v>0</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91">
         <f t="shared" si="2"/>
-        <v>60.664000000000001</v>
+        <v>59.448</v>
       </c>
       <c r="E91">
         <f t="shared" si="3"/>
-        <v>0.13499999999999801</v>
+        <v>0.13600000000000279</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>61610</v>
+        <v>59853</v>
       </c>
       <c r="B92" t="s">
         <v>0</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <f t="shared" si="2"/>
-        <v>61.61</v>
+        <v>59.853000000000002</v>
       </c>
       <c r="E92">
         <f t="shared" si="3"/>
-        <v>0.94599999999999795</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>61745</v>
+        <v>59988</v>
       </c>
       <c r="B93" t="s">
         <v>0</v>
@@ -2641,7 +2650,7 @@
       </c>
       <c r="D93">
         <f t="shared" si="2"/>
-        <v>61.744999999999997</v>
+        <v>59.988</v>
       </c>
       <c r="E93">
         <f t="shared" si="3"/>
@@ -2650,197 +2659,197 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>61880</v>
+        <v>60394</v>
       </c>
       <c r="B94" t="s">
         <v>0</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94">
         <f t="shared" si="2"/>
-        <v>61.88</v>
+        <v>60.393999999999998</v>
       </c>
       <c r="E94">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.40599999999999881</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>62826</v>
+        <v>60529</v>
       </c>
       <c r="B95" t="s">
         <v>0</v>
       </c>
       <c r="C95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D95">
         <f t="shared" si="2"/>
-        <v>62.826000000000001</v>
+        <v>60.529000000000003</v>
       </c>
       <c r="E95">
         <f t="shared" si="3"/>
-        <v>0.94599999999999795</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>63096</v>
+        <v>60664</v>
       </c>
       <c r="B96" t="s">
         <v>0</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D96">
         <f t="shared" si="2"/>
-        <v>63.095999999999997</v>
+        <v>60.664000000000001</v>
       </c>
       <c r="E96">
         <f t="shared" si="3"/>
-        <v>0.26999999999999602</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>63502</v>
+        <v>61610</v>
       </c>
       <c r="B97" t="s">
         <v>0</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97">
         <f t="shared" si="2"/>
-        <v>63.502000000000002</v>
+        <v>61.61</v>
       </c>
       <c r="E97">
         <f t="shared" si="3"/>
-        <v>0.40600000000000591</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>64448</v>
+        <v>61745</v>
       </c>
       <c r="B98" t="s">
         <v>0</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D98">
         <f t="shared" si="2"/>
-        <v>64.447999999999993</v>
+        <v>61.744999999999997</v>
       </c>
       <c r="E98">
         <f t="shared" si="3"/>
-        <v>0.94599999999999085</v>
+        <v>0.13499999999999801</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>64853</v>
+        <v>61880</v>
       </c>
       <c r="B99" t="s">
         <v>0</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99">
         <f t="shared" si="2"/>
-        <v>64.852999999999994</v>
+        <v>61.88</v>
       </c>
       <c r="E99">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>64988</v>
+        <v>62826</v>
       </c>
       <c r="B100" t="s">
         <v>0</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D100">
         <f t="shared" si="2"/>
-        <v>64.988</v>
+        <v>62.826000000000001</v>
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>65123</v>
+        <v>63096</v>
       </c>
       <c r="B101" t="s">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D101">
         <f t="shared" si="2"/>
-        <v>65.123000000000005</v>
+        <v>63.095999999999997</v>
       </c>
       <c r="E101">
         <f t="shared" si="3"/>
-        <v>0.13500000000000512</v>
+        <v>0.26999999999999602</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>65664</v>
+        <v>63502</v>
       </c>
       <c r="B102" t="s">
         <v>0</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102">
         <f t="shared" si="2"/>
-        <v>65.664000000000001</v>
+        <v>63.502000000000002</v>
       </c>
       <c r="E102">
         <f t="shared" si="3"/>
-        <v>0.54099999999999682</v>
+        <v>0.40600000000000591</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>66340</v>
+        <v>64448</v>
       </c>
       <c r="B103" t="s">
         <v>0</v>
       </c>
       <c r="C103">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D103">
         <f t="shared" si="2"/>
-        <v>66.34</v>
+        <v>64.447999999999993</v>
       </c>
       <c r="E103">
         <f t="shared" si="3"/>
-        <v>0.67600000000000193</v>
+        <v>0.94599999999999085</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>66475</v>
+        <v>64853</v>
       </c>
       <c r="B104" t="s">
         <v>0</v>
@@ -2850,54 +2859,54 @@
       </c>
       <c r="D104">
         <f t="shared" si="2"/>
-        <v>66.474999999999994</v>
+        <v>64.852999999999994</v>
       </c>
       <c r="E104">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>66880</v>
+        <v>64988</v>
       </c>
       <c r="B105" t="s">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D105">
         <f t="shared" si="2"/>
-        <v>66.88</v>
+        <v>64.988</v>
       </c>
       <c r="E105">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>67150</v>
+        <v>65123</v>
       </c>
       <c r="B106" t="s">
         <v>0</v>
       </c>
       <c r="C106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D106">
         <f t="shared" si="2"/>
-        <v>67.150000000000006</v>
+        <v>65.123000000000005</v>
       </c>
       <c r="E106">
         <f t="shared" si="3"/>
-        <v>0.27000000000001023</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>68096</v>
+        <v>65664</v>
       </c>
       <c r="B107" t="s">
         <v>0</v>
@@ -2907,54 +2916,54 @@
       </c>
       <c r="D107">
         <f t="shared" si="2"/>
-        <v>68.096000000000004</v>
+        <v>65.664000000000001</v>
       </c>
       <c r="E107">
         <f t="shared" si="3"/>
-        <v>0.94599999999999795</v>
+        <v>0.54099999999999682</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>68231</v>
+        <v>66340</v>
       </c>
       <c r="B108" t="s">
         <v>0</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108">
         <f t="shared" si="2"/>
-        <v>68.230999999999995</v>
+        <v>66.34</v>
       </c>
       <c r="E108">
         <f t="shared" si="3"/>
-        <v>0.13499999999999091</v>
+        <v>0.67600000000000193</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>68367</v>
+        <v>66475</v>
       </c>
       <c r="B109" t="s">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D109">
         <f t="shared" si="2"/>
-        <v>68.367000000000004</v>
+        <v>66.474999999999994</v>
       </c>
       <c r="E109">
         <f t="shared" si="3"/>
-        <v>0.13600000000000989</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>69312</v>
+        <v>66880</v>
       </c>
       <c r="B110" t="s">
         <v>0</v>
@@ -2964,16 +2973,16 @@
       </c>
       <c r="D110">
         <f t="shared" si="2"/>
-        <v>69.311999999999998</v>
+        <v>66.88</v>
       </c>
       <c r="E110">
         <f t="shared" si="3"/>
-        <v>0.94499999999999318</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>69583</v>
+        <v>67150</v>
       </c>
       <c r="B111" t="s">
         <v>0</v>
@@ -2983,35 +2992,35 @@
       </c>
       <c r="D111">
         <f t="shared" si="2"/>
-        <v>69.582999999999998</v>
+        <v>67.150000000000006</v>
       </c>
       <c r="E111">
         <f t="shared" si="3"/>
-        <v>0.2710000000000008</v>
+        <v>0.27000000000001023</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>69988</v>
+        <v>68096</v>
       </c>
       <c r="B112" t="s">
         <v>0</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D112">
         <f t="shared" si="2"/>
-        <v>69.988</v>
+        <v>68.096000000000004</v>
       </c>
       <c r="E112">
         <f t="shared" si="3"/>
-        <v>0.40500000000000114</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>70934</v>
+        <v>68231</v>
       </c>
       <c r="B113" t="s">
         <v>0</v>
@@ -3021,178 +3030,178 @@
       </c>
       <c r="D113">
         <f t="shared" si="2"/>
-        <v>70.933999999999997</v>
+        <v>68.230999999999995</v>
       </c>
       <c r="E113">
         <f t="shared" si="3"/>
-        <v>0.94599999999999795</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>71340</v>
+        <v>68367</v>
       </c>
       <c r="B114" t="s">
         <v>0</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D114">
         <f t="shared" si="2"/>
-        <v>71.34</v>
+        <v>68.367000000000004</v>
       </c>
       <c r="E114">
         <f t="shared" si="3"/>
-        <v>0.40600000000000591</v>
+        <v>0.13600000000000989</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>72015</v>
+        <v>69312</v>
       </c>
       <c r="B115" t="s">
         <v>0</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D115">
-        <f t="shared" ref="D115:D165" si="4">A115/1000</f>
-        <v>72.015000000000001</v>
+        <f t="shared" si="2"/>
+        <v>69.311999999999998</v>
       </c>
       <c r="E115">
         <f t="shared" si="3"/>
-        <v>0.67499999999999716</v>
+        <v>0.94499999999999318</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
+        <v>69583</v>
+      </c>
+      <c r="B116" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="2"/>
+        <v>69.582999999999998</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="3"/>
+        <v>0.2710000000000008</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>69988</v>
+      </c>
+      <c r="B117" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="2"/>
+        <v>69.988</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="3"/>
+        <v>0.40500000000000114</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>70934</v>
+      </c>
+      <c r="B118" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="2"/>
+        <v>70.933999999999997</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="3"/>
+        <v>0.94599999999999795</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>71340</v>
+      </c>
+      <c r="B119" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="2"/>
+        <v>71.34</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="3"/>
+        <v>0.40600000000000591</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>72015</v>
+      </c>
+      <c r="B120" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <f t="shared" ref="D120:D171" si="4">A120/1000</f>
+        <v>72.015000000000001</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="3"/>
+        <v>0.67499999999999716</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
         <v>72826</v>
       </c>
-      <c r="B116" t="s">
-        <v>0</v>
-      </c>
-      <c r="C116">
-        <v>2</v>
-      </c>
-      <c r="D116">
+      <c r="B121" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121">
         <f t="shared" si="4"/>
         <v>72.825999999999993</v>
       </c>
-      <c r="E116">
-        <f t="shared" ref="E116:E165" si="5">D116-D115</f>
+      <c r="E121">
+        <f t="shared" ref="E121:E171" si="5">D121-D120</f>
         <v>0.81099999999999284</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
         <v>72961</v>
       </c>
-      <c r="B117" t="s">
-        <v>0</v>
-      </c>
-      <c r="C117">
-        <v>2</v>
-      </c>
-      <c r="D117">
+      <c r="B122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122">
         <f t="shared" si="4"/>
         <v>72.960999999999999</v>
-      </c>
-      <c r="E117">
-        <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118">
-        <v>73367</v>
-      </c>
-      <c r="B118" t="s">
-        <v>0</v>
-      </c>
-      <c r="C118">
-        <v>1</v>
-      </c>
-      <c r="D118">
-        <f t="shared" si="4"/>
-        <v>73.367000000000004</v>
-      </c>
-      <c r="E118">
-        <f t="shared" si="5"/>
-        <v>0.40600000000000591</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>73502</v>
-      </c>
-      <c r="B119" t="s">
-        <v>0</v>
-      </c>
-      <c r="C119">
-        <v>1</v>
-      </c>
-      <c r="D119">
-        <f t="shared" si="4"/>
-        <v>73.501999999999995</v>
-      </c>
-      <c r="E119">
-        <f t="shared" si="5"/>
-        <v>0.13499999999999091</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>73637</v>
-      </c>
-      <c r="B120" t="s">
-        <v>0</v>
-      </c>
-      <c r="C120">
-        <v>1</v>
-      </c>
-      <c r="D120">
-        <f t="shared" si="4"/>
-        <v>73.637</v>
-      </c>
-      <c r="E120">
-        <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>74583</v>
-      </c>
-      <c r="B121" t="s">
-        <v>0</v>
-      </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-      <c r="D121">
-        <f t="shared" si="4"/>
-        <v>74.582999999999998</v>
-      </c>
-      <c r="E121">
-        <f t="shared" si="5"/>
-        <v>0.94599999999999795</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>74718</v>
-      </c>
-      <c r="B122" t="s">
-        <v>0</v>
-      </c>
-      <c r="C122">
-        <v>0</v>
-      </c>
-      <c r="D122">
-        <f t="shared" si="4"/>
-        <v>74.718000000000004</v>
       </c>
       <c r="E122">
         <f t="shared" si="5"/>
@@ -3201,26 +3210,26 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>74853</v>
+        <v>73367</v>
       </c>
       <c r="B123" t="s">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D123">
         <f t="shared" si="4"/>
-        <v>74.852999999999994</v>
+        <v>73.367000000000004</v>
       </c>
       <c r="E123">
         <f t="shared" si="5"/>
-        <v>0.13499999999999091</v>
+        <v>0.40600000000000591</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>75394</v>
+        <v>73502</v>
       </c>
       <c r="B124" t="s">
         <v>0</v>
@@ -3230,282 +3239,282 @@
       </c>
       <c r="D124">
         <f t="shared" si="4"/>
-        <v>75.394000000000005</v>
+        <v>73.501999999999995</v>
       </c>
       <c r="E124">
         <f t="shared" si="5"/>
-        <v>0.54100000000001103</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>76204</v>
+        <v>73637</v>
       </c>
       <c r="B125" t="s">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D125">
         <f t="shared" si="4"/>
-        <v>76.203999999999994</v>
+        <v>73.637</v>
       </c>
       <c r="E125">
         <f t="shared" si="5"/>
-        <v>0.80999999999998806</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>76340</v>
+        <v>74583</v>
       </c>
       <c r="B126" t="s">
         <v>0</v>
       </c>
       <c r="C126">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D126">
         <f t="shared" si="4"/>
-        <v>76.34</v>
+        <v>74.582999999999998</v>
       </c>
       <c r="E126">
         <f t="shared" si="5"/>
-        <v>0.13600000000000989</v>
+        <v>0.94599999999999795</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>76475</v>
+        <v>74718</v>
       </c>
       <c r="B127" t="s">
         <v>0</v>
       </c>
       <c r="C127">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D127">
         <f t="shared" si="4"/>
-        <v>76.474999999999994</v>
+        <v>74.718000000000004</v>
       </c>
       <c r="E127">
         <f t="shared" si="5"/>
-        <v>0.13499999999999091</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>77015</v>
+        <v>74853</v>
       </c>
       <c r="B128" t="s">
         <v>0</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128">
         <f t="shared" si="4"/>
-        <v>77.015000000000001</v>
+        <v>74.852999999999994</v>
       </c>
       <c r="E128">
         <f t="shared" si="5"/>
-        <v>0.54000000000000625</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>77826</v>
+        <v>75394</v>
       </c>
       <c r="B129" t="s">
         <v>0</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129">
         <f t="shared" si="4"/>
-        <v>77.825999999999993</v>
+        <v>75.394000000000005</v>
       </c>
       <c r="E129">
         <f t="shared" si="5"/>
-        <v>0.81099999999999284</v>
+        <v>0.54100000000001103</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>77961</v>
+        <v>76204</v>
       </c>
       <c r="B130" t="s">
         <v>0</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D130">
         <f t="shared" si="4"/>
-        <v>77.960999999999999</v>
+        <v>76.203999999999994</v>
       </c>
       <c r="E130">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.80999999999998806</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>78096</v>
+        <v>76340</v>
       </c>
       <c r="B131" t="s">
         <v>0</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D131">
         <f t="shared" si="4"/>
-        <v>78.096000000000004</v>
+        <v>76.34</v>
       </c>
       <c r="E131">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.13600000000000989</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>78637</v>
+        <v>76475</v>
       </c>
       <c r="B132" t="s">
         <v>0</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D132">
         <f t="shared" si="4"/>
-        <v>78.637</v>
+        <v>76.474999999999994</v>
       </c>
       <c r="E132">
         <f t="shared" si="5"/>
-        <v>0.54099999999999682</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>78907</v>
+        <v>77015</v>
       </c>
       <c r="B133" t="s">
         <v>0</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D133">
         <f t="shared" si="4"/>
-        <v>78.906999999999996</v>
+        <v>77.015000000000001</v>
       </c>
       <c r="E133">
         <f t="shared" si="5"/>
-        <v>0.26999999999999602</v>
+        <v>0.54000000000000625</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>79312</v>
+        <v>77826</v>
       </c>
       <c r="B134" t="s">
         <v>0</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D134">
         <f t="shared" si="4"/>
-        <v>79.311999999999998</v>
+        <v>77.825999999999993</v>
       </c>
       <c r="E134">
         <f t="shared" si="5"/>
-        <v>0.40500000000000114</v>
+        <v>0.81099999999999284</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>79448</v>
+        <v>77961</v>
       </c>
       <c r="B135" t="s">
         <v>0</v>
       </c>
       <c r="C135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D135">
         <f t="shared" si="4"/>
-        <v>79.447999999999993</v>
+        <v>77.960999999999999</v>
       </c>
       <c r="E135">
         <f t="shared" si="5"/>
-        <v>0.13599999999999568</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>81069</v>
+        <v>78096</v>
       </c>
       <c r="B136" t="s">
         <v>0</v>
       </c>
       <c r="C136">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D136">
         <f t="shared" si="4"/>
-        <v>81.069000000000003</v>
+        <v>78.096000000000004</v>
       </c>
       <c r="E136">
         <f t="shared" si="5"/>
-        <v>1.6210000000000093</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>81204</v>
+        <v>78637</v>
       </c>
       <c r="B137" t="s">
         <v>0</v>
       </c>
       <c r="C137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D137">
         <f t="shared" si="4"/>
-        <v>81.203999999999994</v>
+        <v>78.637</v>
       </c>
       <c r="E137">
         <f t="shared" si="5"/>
-        <v>0.13499999999999091</v>
+        <v>0.54099999999999682</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>81340</v>
+        <v>78907</v>
       </c>
       <c r="B138" t="s">
         <v>0</v>
       </c>
       <c r="C138">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D138">
         <f t="shared" si="4"/>
-        <v>81.34</v>
+        <v>78.906999999999996</v>
       </c>
       <c r="E138">
         <f t="shared" si="5"/>
-        <v>0.13600000000000989</v>
+        <v>0.26999999999999602</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>81880</v>
+        <v>79312</v>
       </c>
       <c r="B139" t="s">
         <v>0</v>
@@ -3515,16 +3524,16 @@
       </c>
       <c r="D139">
         <f t="shared" si="4"/>
-        <v>81.88</v>
+        <v>79.311999999999998</v>
       </c>
       <c r="E139">
         <f t="shared" si="5"/>
-        <v>0.53999999999999204</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>82015</v>
+        <v>79448</v>
       </c>
       <c r="B140" t="s">
         <v>0</v>
@@ -3534,168 +3543,168 @@
       </c>
       <c r="D140">
         <f t="shared" si="4"/>
-        <v>82.015000000000001</v>
+        <v>79.447999999999993</v>
       </c>
       <c r="E140">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.13599999999999568</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>82150</v>
+        <v>81069</v>
       </c>
       <c r="B141" t="s">
         <v>0</v>
       </c>
       <c r="C141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D141">
         <f t="shared" si="4"/>
-        <v>82.15</v>
+        <v>81.069000000000003</v>
       </c>
       <c r="E141">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>1.6210000000000093</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>82691</v>
+        <v>81204</v>
       </c>
       <c r="B142" t="s">
         <v>0</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D142">
         <f t="shared" si="4"/>
-        <v>82.691000000000003</v>
+        <v>81.203999999999994</v>
       </c>
       <c r="E142">
         <f t="shared" si="5"/>
-        <v>0.54099999999999682</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>82826</v>
+        <v>81340</v>
       </c>
       <c r="B143" t="s">
         <v>0</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D143">
         <f t="shared" si="4"/>
-        <v>82.825999999999993</v>
+        <v>81.34</v>
       </c>
       <c r="E143">
         <f t="shared" si="5"/>
-        <v>0.13499999999999091</v>
+        <v>0.13600000000000989</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>82961</v>
+        <v>81880</v>
       </c>
       <c r="B144" t="s">
         <v>0</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D144">
         <f t="shared" si="4"/>
-        <v>82.960999999999999</v>
+        <v>81.88</v>
       </c>
       <c r="E144">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.53999999999999204</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>83772</v>
+        <v>82015</v>
       </c>
       <c r="B145" t="s">
         <v>0</v>
       </c>
       <c r="C145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D145">
         <f t="shared" si="4"/>
-        <v>83.772000000000006</v>
+        <v>82.015000000000001</v>
       </c>
       <c r="E145">
         <f t="shared" si="5"/>
-        <v>0.81100000000000705</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>83907</v>
+        <v>82150</v>
       </c>
       <c r="B146" t="s">
         <v>0</v>
       </c>
       <c r="C146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146">
         <f t="shared" si="4"/>
-        <v>83.906999999999996</v>
+        <v>82.15</v>
       </c>
       <c r="E146">
         <f t="shared" si="5"/>
-        <v>0.13499999999999091</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>84312</v>
+        <v>82691</v>
       </c>
       <c r="B147" t="s">
         <v>0</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147">
         <f t="shared" si="4"/>
-        <v>84.311999999999998</v>
+        <v>82.691000000000003</v>
       </c>
       <c r="E147">
         <f t="shared" si="5"/>
-        <v>0.40500000000000114</v>
+        <v>0.54099999999999682</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>85123</v>
+        <v>82826</v>
       </c>
       <c r="B148" t="s">
         <v>0</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D148">
         <f t="shared" si="4"/>
-        <v>85.123000000000005</v>
+        <v>82.825999999999993</v>
       </c>
       <c r="E148">
         <f t="shared" si="5"/>
-        <v>0.81100000000000705</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>85934</v>
+        <v>82961</v>
       </c>
       <c r="B149" t="s">
         <v>0</v>
@@ -3705,35 +3714,35 @@
       </c>
       <c r="D149">
         <f t="shared" si="4"/>
-        <v>85.933999999999997</v>
+        <v>82.960999999999999</v>
       </c>
       <c r="E149">
         <f t="shared" si="5"/>
-        <v>0.81099999999999284</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>86204</v>
+        <v>83772</v>
       </c>
       <c r="B150" t="s">
         <v>0</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D150">
         <f t="shared" si="4"/>
-        <v>86.203999999999994</v>
+        <v>83.772000000000006</v>
       </c>
       <c r="E150">
         <f t="shared" si="5"/>
-        <v>0.26999999999999602</v>
+        <v>0.81100000000000705</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>87556</v>
+        <v>83907</v>
       </c>
       <c r="B151" t="s">
         <v>0</v>
@@ -3743,35 +3752,35 @@
       </c>
       <c r="D151">
         <f t="shared" si="4"/>
-        <v>87.555999999999997</v>
+        <v>83.906999999999996</v>
       </c>
       <c r="E151">
         <f t="shared" si="5"/>
-        <v>1.3520000000000039</v>
+        <v>0.13499999999999091</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>87691</v>
+        <v>84312</v>
       </c>
       <c r="B152" t="s">
         <v>0</v>
       </c>
       <c r="C152">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D152">
         <f t="shared" si="4"/>
-        <v>87.691000000000003</v>
+        <v>84.311999999999998</v>
       </c>
       <c r="E152">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.40500000000000114</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>87826</v>
+        <v>85123</v>
       </c>
       <c r="B153" t="s">
         <v>0</v>
@@ -3781,16 +3790,16 @@
       </c>
       <c r="D153">
         <f t="shared" si="4"/>
-        <v>87.825999999999993</v>
+        <v>85.123000000000005</v>
       </c>
       <c r="E153">
         <f t="shared" si="5"/>
-        <v>0.13499999999999091</v>
+        <v>0.81100000000000705</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>88772</v>
+        <v>85934</v>
       </c>
       <c r="B154" t="s">
         <v>0</v>
@@ -3800,16 +3809,16 @@
       </c>
       <c r="D154">
         <f t="shared" si="4"/>
-        <v>88.772000000000006</v>
+        <v>85.933999999999997</v>
       </c>
       <c r="E154">
         <f t="shared" si="5"/>
-        <v>0.94600000000001216</v>
+        <v>0.81099999999999284</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>89042</v>
+        <v>86204</v>
       </c>
       <c r="B155" t="s">
         <v>0</v>
@@ -3819,7 +3828,7 @@
       </c>
       <c r="D155">
         <f t="shared" si="4"/>
-        <v>89.042000000000002</v>
+        <v>86.203999999999994</v>
       </c>
       <c r="E155">
         <f t="shared" si="5"/>
@@ -3828,26 +3837,26 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>89448</v>
+        <v>87556</v>
       </c>
       <c r="B156" t="s">
         <v>0</v>
       </c>
       <c r="C156">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D156">
         <f t="shared" si="4"/>
-        <v>89.447999999999993</v>
+        <v>87.555999999999997</v>
       </c>
       <c r="E156">
         <f t="shared" si="5"/>
-        <v>0.4059999999999917</v>
+        <v>1.3520000000000039</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>90394</v>
+        <v>87691</v>
       </c>
       <c r="B157" t="s">
         <v>0</v>
@@ -3857,16 +3866,16 @@
       </c>
       <c r="D157">
         <f t="shared" si="4"/>
-        <v>90.394000000000005</v>
+        <v>87.691000000000003</v>
       </c>
       <c r="E157">
         <f t="shared" si="5"/>
-        <v>0.94600000000001216</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>90529</v>
+        <v>87826</v>
       </c>
       <c r="B158" t="s">
         <v>0</v>
@@ -3876,7 +3885,7 @@
       </c>
       <c r="D158">
         <f t="shared" si="4"/>
-        <v>90.528999999999996</v>
+        <v>87.825999999999993</v>
       </c>
       <c r="E158">
         <f t="shared" si="5"/>
@@ -3885,93 +3894,93 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>90664</v>
+        <v>88772</v>
       </c>
       <c r="B159" t="s">
         <v>0</v>
       </c>
       <c r="C159">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D159">
         <f t="shared" si="4"/>
-        <v>90.664000000000001</v>
+        <v>88.772000000000006</v>
       </c>
       <c r="E159">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.94600000000001216</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>90799</v>
+        <v>89042</v>
       </c>
       <c r="B160" t="s">
         <v>0</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D160">
         <f t="shared" si="4"/>
-        <v>90.799000000000007</v>
+        <v>89.042000000000002</v>
       </c>
       <c r="E160">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.26999999999999602</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>91610</v>
+        <v>89448</v>
       </c>
       <c r="B161" t="s">
         <v>0</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D161">
         <f t="shared" si="4"/>
-        <v>91.61</v>
+        <v>89.447999999999993</v>
       </c>
       <c r="E161">
         <f t="shared" si="5"/>
-        <v>0.81099999999999284</v>
+        <v>0.4059999999999917</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>91745</v>
+        <v>90394</v>
       </c>
       <c r="B162" t="s">
         <v>0</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D162">
         <f t="shared" si="4"/>
-        <v>91.745000000000005</v>
+        <v>90.394000000000005</v>
       </c>
       <c r="E162">
         <f t="shared" si="5"/>
-        <v>0.13500000000000512</v>
+        <v>0.94600000000001216</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>91880</v>
+        <v>90529</v>
       </c>
       <c r="B163" t="s">
         <v>0</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D163">
         <f t="shared" si="4"/>
-        <v>91.88</v>
+        <v>90.528999999999996</v>
       </c>
       <c r="E163">
         <f t="shared" si="5"/>
@@ -3980,40 +3989,154 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>92285</v>
+        <v>90664</v>
       </c>
       <c r="B164" t="s">
         <v>0</v>
       </c>
       <c r="C164">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D164">
         <f t="shared" si="4"/>
-        <v>92.284999999999997</v>
+        <v>90.664000000000001</v>
       </c>
       <c r="E164">
         <f t="shared" si="5"/>
-        <v>0.40500000000000114</v>
+        <v>0.13500000000000512</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>92421</v>
+        <v>90799</v>
       </c>
       <c r="B165" t="s">
         <v>0</v>
       </c>
       <c r="C165">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D165">
         <f t="shared" si="4"/>
-        <v>92.421000000000006</v>
+        <v>90.799000000000007</v>
       </c>
       <c r="E165">
         <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>91610</v>
+      </c>
+      <c r="B166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166">
+        <f t="shared" si="4"/>
+        <v>91.61</v>
+      </c>
+      <c r="E166">
+        <f t="shared" si="5"/>
+        <v>0.81099999999999284</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>91745</v>
+      </c>
+      <c r="B167" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
+      <c r="D167">
+        <f t="shared" si="4"/>
+        <v>91.745000000000005</v>
+      </c>
+      <c r="E167">
+        <f t="shared" si="5"/>
+        <v>0.13500000000000512</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>91880</v>
+      </c>
+      <c r="B168" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <f t="shared" si="4"/>
+        <v>91.88</v>
+      </c>
+      <c r="E168">
+        <f t="shared" si="5"/>
+        <v>0.13499999999999091</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>92285</v>
+      </c>
+      <c r="B169" t="s">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <f t="shared" si="4"/>
+        <v>92.284999999999997</v>
+      </c>
+      <c r="E169">
+        <f t="shared" si="5"/>
+        <v>0.40500000000000114</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>92421</v>
+      </c>
+      <c r="B170" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <f t="shared" si="4"/>
+        <v>92.421000000000006</v>
+      </c>
+      <c r="E170">
+        <f t="shared" si="5"/>
         <v>0.13600000000000989</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>93500</v>
+      </c>
+      <c r="B171" t="s">
+        <v>2</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <f t="shared" si="4"/>
+        <v>93.5</v>
+      </c>
+      <c r="E171">
+        <f t="shared" si="5"/>
+        <v>1.0789999999999935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>